<commit_message>
cabaña se puede entrar por id, falta ruta
</commit_message>
<xml_diff>
--- a/cabaniapp/Requisitos pig.xlsx
+++ b/cabaniapp/Requisitos pig.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>● El PIG debe subirse a un repositorio GIT público en la nube.</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>principal y perfil?</t>
+  </si>
+  <si>
+    <t>las cabañas se puede entrar por id</t>
   </si>
 </sst>
 </file>
@@ -189,13 +192,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,28 +528,31 @@
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -619,10 +625,10 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="3" t="s">
         <v>24</v>
       </c>
@@ -643,10 +649,10 @@
       <c r="C22" s="6"/>
     </row>
     <row r="24" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="9"/>
       <c r="D24" t="s">
         <v>28</v>
       </c>

</xml_diff>